<commit_message>
Automatische test-sync: 2025-06-27 00:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -722,8 +722,59 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun je deze taak op je nemen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #20: Kun je deze taak op je nemen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Bedankt voor je bericht. Kun je wat meer details geven over welke taak je precies bedoelt? Dan kan ik je zo goed mogelijk helpen.
+Met vriendelijke groet,
+[Jouw naam]  
+E-mailassistent bij [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-27 00:03:01</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -743,7 +794,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -751,12 +802,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -771,7 +822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -801,6 +852,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:14:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -773,8 +773,58 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:14:36</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -794,7 +844,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -802,12 +852,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,7 +872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -862,6 +912,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,8 +823,58 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:19:31</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -844,7 +894,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -852,12 +902,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -895,17 +945,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -915,7 +965,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,8 +873,58 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:24:11</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -894,7 +944,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -902,12 +952,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -949,7 +999,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -923,8 +923,58 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:28:38</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -944,7 +994,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -952,12 +1002,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -999,7 +1049,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -973,8 +973,58 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:36:39</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -994,7 +1044,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1002,12 +1052,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1049,7 +1099,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1023,8 +1023,58 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:38:47</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1044,7 +1094,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1052,12 +1102,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1099,7 +1149,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1073,8 +1073,58 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:42:34</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1094,7 +1144,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1102,12 +1152,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1149,7 +1199,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1123,8 +1123,60 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Helaas kan ik geen bestellingen plaatsen, maar ik kan u doorverwijzen naar het bestelteam binnen ons bedrijf. Graag ontvang ik de contactgegevens van uw bedrijf, zodat ik de juiste persoon met u in contact kan brengen.
+Ik zie uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:44:46</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1144,7 +1196,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1152,12 +1204,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1172,7 +1224,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,6 +1274,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1175,8 +1175,59 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #3: Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank u voor uw interesse in onze producten/diensten. Om u nauwkeurige informatie te verstrekken over de verzendkosten, hebben we meer details nodig zoals het product/dienst waar u naar informeert en het afleveradres. Zou u ons kunnen voorzien van deze informatie zodat we u een precieze schatting van de verzendkosten kunnen geven?
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:46:58</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1196,7 +1247,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1204,12 +1255,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1224,7 +1275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1284,6 +1335,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-27 22:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-27.xlsx
+++ b/logs/mail_log_2025-06-27.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1226,8 +1226,59 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je interesse in ons artikel. Helaas kan ik je op basis van dit bericht niet verder helpen. Kun je meer details geven over welk artikel je wilt inkopen en op welke manier? Zo kan ik je beter assisteren.
+Met vriendelijke groet,
+[Jouw naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-27 22:49:08</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1247,7 +1298,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1255,12 +1306,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1308,17 +1359,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1328,7 +1379,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>